<commit_message>
longest common subsequence added in Dynamic
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABHI\jupyter notebook\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114A8BE1-E362-4958-AAB8-5EC3F8B9990D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A103FD-19B7-4CBC-B491-15DAA86327DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5736" yWindow="348" windowWidth="17280" windowHeight="8964" tabRatio="145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2776" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2777" uniqueCount="483">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1471,6 +1471,9 @@
   </si>
   <si>
     <t>This sheet is taken from</t>
+  </si>
+  <si>
+    <t>more about subsequences in Dynamic DSA.ipynb</t>
   </si>
 </sst>
 </file>
@@ -1919,10 +1922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H481"/>
+  <dimension ref="A1:I481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A405" zoomScale="72" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C409" sqref="C409"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3440,7 +3443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="21">
+    <row r="65" spans="1:9" ht="21">
       <c r="A65" s="5" t="s">
         <v>52</v>
       </c>
@@ -3465,8 +3468,11 @@
       <c r="H65" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" ht="21">
+      <c r="I65" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="21">
       <c r="A66" s="5" t="s">
         <v>52</v>
       </c>
@@ -3492,7 +3498,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="21">
+    <row r="67" spans="1:9" ht="21">
       <c r="A67" s="5" t="s">
         <v>52</v>
       </c>
@@ -3518,7 +3524,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="21">
+    <row r="68" spans="1:9" ht="21">
       <c r="A68" s="5" t="s">
         <v>52</v>
       </c>
@@ -3544,7 +3550,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="21">
+    <row r="69" spans="1:9" ht="21">
       <c r="A69" s="5" t="s">
         <v>52</v>
       </c>
@@ -3570,7 +3576,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="21">
+    <row r="70" spans="1:9" ht="21">
       <c r="A70" s="5" t="s">
         <v>52</v>
       </c>
@@ -3596,7 +3602,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="21">
+    <row r="71" spans="1:9" ht="21">
       <c r="A71" s="5" t="s">
         <v>52</v>
       </c>
@@ -3622,7 +3628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="21">
+    <row r="72" spans="1:9" ht="21">
       <c r="A72" s="5" t="s">
         <v>52</v>
       </c>
@@ -3648,7 +3654,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="21">
+    <row r="73" spans="1:9" ht="21">
       <c r="A73" s="5" t="s">
         <v>52</v>
       </c>
@@ -3674,7 +3680,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="21">
+    <row r="74" spans="1:9" ht="21">
       <c r="A74" s="5" t="s">
         <v>52</v>
       </c>
@@ -3700,7 +3706,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="21">
+    <row r="75" spans="1:9" ht="21">
       <c r="A75" s="5" t="s">
         <v>52</v>
       </c>
@@ -3726,7 +3732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="21">
+    <row r="76" spans="1:9" ht="21">
       <c r="A76" s="5" t="s">
         <v>52</v>
       </c>
@@ -3752,7 +3758,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="21">
+    <row r="77" spans="1:9" ht="21">
       <c r="A77" s="5" t="s">
         <v>52</v>
       </c>
@@ -3778,7 +3784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="21">
+    <row r="78" spans="1:9" ht="21">
       <c r="A78" s="5" t="s">
         <v>52</v>
       </c>
@@ -3804,7 +3810,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="21">
+    <row r="79" spans="1:9" ht="21">
       <c r="A79" s="5" t="s">
         <v>52</v>
       </c>
@@ -3830,7 +3836,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="21">
+    <row r="80" spans="1:9" ht="21">
       <c r="A80" s="5" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
min operations to insertion/deletion to get other string
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABHI\jupyter notebook\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A857F617-BCFB-4830-B9CB-3793E9927662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBCEE47-2203-40A7-85E4-38DF871E1F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1924,8 +1924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A448" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C454" sqref="C454"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>

</xml_diff>

<commit_message>
matrix chain multiplication in Dynamic using recurssion + bottom up
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABHI\jupyter notebook\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4685F336-86D8-49A6-9A6C-AA47E2B3D85C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DB3571-32C9-4BB9-B3F8-AF0FE0FFE159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1924,8 +1924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A445" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F449" sqref="F449"/>
+    <sheetView tabSelected="1" topLeftCell="A401" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C409" sqref="C409"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>

</xml_diff>

<commit_message>
diameter of binary tree
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABHI\jupyter notebook\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC6C24F-6894-48B9-A33F-7FBAAAABA594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4D1446-9CB8-4295-A435-EB8B6A28410D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2760" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2757" uniqueCount="483">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1924,8 +1924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A422" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C431" sqref="C431"/>
+    <sheetView tabSelected="1" topLeftCell="A166" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C187" sqref="C187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -6316,14 +6316,14 @@
       <c r="C180" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="D180" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E180" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F180" s="4" t="s">
-        <v>3</v>
+      <c r="D180" s="4">
+        <v>1</v>
+      </c>
+      <c r="E180" s="4">
+        <v>1</v>
+      </c>
+      <c r="F180" s="4">
+        <v>1</v>
       </c>
       <c r="G180" s="4" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Max sum path binary tree leetcode
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABHI\jupyter notebook\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4D1446-9CB8-4295-A435-EB8B6A28410D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3418011C-E036-4B14-9131-4DEF29FCDF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2757" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2754" uniqueCount="484">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1474,6 +1474,9 @@
   </si>
   <si>
     <t>more about subsequences in Dynamic DSA.ipynb</t>
+  </si>
+  <si>
+    <t>TLE on GFG</t>
   </si>
 </sst>
 </file>
@@ -1924,8 +1927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C187" sqref="C187"/>
+    <sheetView tabSelected="1" topLeftCell="A188" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C202" sqref="C202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -13305,20 +13308,20 @@
       <c r="C460" s="6" t="s">
         <v>442</v>
       </c>
-      <c r="D460" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E460" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F460" s="4" t="s">
-        <v>3</v>
+      <c r="D460" s="4">
+        <v>1</v>
+      </c>
+      <c r="E460" s="4">
+        <v>1</v>
+      </c>
+      <c r="F460" s="4">
+        <v>1</v>
       </c>
       <c r="G460" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H460" s="4" t="s">
-        <v>3</v>
+        <v>483</v>
       </c>
     </row>
     <row r="461" spans="1:8" ht="21">

</xml_diff>

<commit_message>
Leetcode 75, 1122, 215
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABHI\jupyter notebook\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C41706E-7DD2-4E0F-B6DF-CCB629EB8555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658AF7DA-5448-46A1-9687-293C24B2132B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4182" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2091" uniqueCount="480">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1916,7 +1916,7 @@
   <dimension ref="A1:I481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
Leetcode 2149 and sets operations
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABHI\jupyter notebook\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658AF7DA-5448-46A1-9687-293C24B2132B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9A0893-301F-4E5A-A000-D778B61B73FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2091" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4182" uniqueCount="480">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1916,7 +1917,7 @@
   <dimension ref="A1:I481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2034,6 +2035,9 @@
       <c r="F8" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="21">
       <c r="A9" s="5" t="s">
@@ -2054,6 +2058,9 @@
       <c r="F9" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="21">
       <c r="A10" s="5" t="s">
@@ -2073,6 +2080,9 @@
       </c>
       <c r="F10" s="4" t="s">
         <v>3</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="21">

</xml_diff>